<commit_message>
Additional test assertions when autofilter structure is defined in the worksheet file
</commit_message>
<xml_diff>
--- a/tests/data/Features/AutoFilter/Xlsx/AutoFilter_Basic.xlsx
+++ b/tests/data/Features/AutoFilter/Xlsx/AutoFilter_Basic.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0000911A-F39A-48AB-BE50-833AEE0FDA7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Worksheet'!$A$1:$D$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$D$57</definedName>
   </definedNames>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="999999"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="15">
   <si>
     <t>Year</t>
   </si>
@@ -67,23 +73,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -94,31 +92,38 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,19 +413,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -448,7 +451,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2010</v>
       </c>
@@ -462,7 +465,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -476,7 +479,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -490,7 +493,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -504,7 +507,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -518,7 +521,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -532,7 +535,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -546,7 +549,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -560,7 +563,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -574,7 +577,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -588,7 +591,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2010</v>
       </c>
@@ -602,7 +605,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -616,7 +619,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -630,7 +633,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -644,7 +647,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -658,7 +661,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2010</v>
       </c>
@@ -672,7 +675,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2010</v>
       </c>
@@ -686,7 +689,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2010</v>
       </c>
@@ -700,7 +703,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2010</v>
       </c>
@@ -714,7 +717,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -728,7 +731,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -742,7 +745,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -756,7 +759,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -770,7 +773,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2010</v>
       </c>
@@ -784,7 +787,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2010</v>
       </c>
@@ -798,7 +801,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2010</v>
       </c>
@@ -812,7 +815,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2010</v>
       </c>
@@ -826,7 +829,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -840,7 +843,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -854,7 +857,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2011</v>
       </c>
@@ -868,7 +871,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -882,7 +885,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2010</v>
       </c>
@@ -896,7 +899,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2010</v>
       </c>
@@ -910,7 +913,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2010</v>
       </c>
@@ -924,7 +927,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2010</v>
       </c>
@@ -938,7 +941,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2011</v>
       </c>
@@ -952,7 +955,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -966,7 +969,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2011</v>
       </c>
@@ -980,7 +983,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2011</v>
       </c>
@@ -994,7 +997,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2010</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2010</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2010</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2011</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2011</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2011</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2011</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2010</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2010</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2010</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2010</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2011</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2011</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2011</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2011</v>
       </c>
@@ -1219,18 +1222,21 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <autoFilter ref="A1:D57"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <autoFilter ref="A1:D57" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="UK"/>
+        <filter val="United States"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <customFilters and="1">
+        <customFilter operator="greaterThan" val="650"/>
+        <customFilter operator="lessThan" val="800"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>